<commit_message>
Change: All dimensions consistent to DDL Thesis
</commit_message>
<xml_diff>
--- a/Dimensions/Dimensions.xlsx
+++ b/Dimensions/Dimensions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="150" windowWidth="14355" windowHeight="2895"/>
+    <workbookView xWindow="360" yWindow="270" windowWidth="14355" windowHeight="2775"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,8 +15,90 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Troy Haskin</author>
+  </authors>
+  <commentList>
+    <comment ref="K5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Troy Haskin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+From Darius's CAD model.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Troy Haskin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+From Darius's CAD model</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Troy Haskin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+To ensure the loop is closed (to within roundoff), the derived measures will be used, but these measurements show how far the derived lengths are from those pictured.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="35">
   <si>
     <t>From</t>
   </si>
@@ -57,13 +139,7 @@
     <t>Hot Inlet CL</t>
   </si>
   <si>
-    <t>Picutred</t>
-  </si>
-  <si>
     <t>Derived</t>
-  </si>
-  <si>
-    <t>Cap Radius</t>
   </si>
   <si>
     <t>Tee Volume</t>
@@ -74,6 +150,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <vertAlign val="superscript"/>
         <sz val="11"/>
         <color theme="1"/>
@@ -90,6 +167,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <vertAlign val="superscript"/>
         <sz val="11"/>
         <color theme="1"/>
@@ -100,15 +178,69 @@
       <t>3</t>
     </r>
   </si>
+  <si>
+    <t>Water Fill Heights</t>
+  </si>
+  <si>
+    <t>Fill [%]</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Tank Cylinder Bottom</t>
+  </si>
+  <si>
+    <t>Tank Cylinder Top</t>
+  </si>
+  <si>
+    <t>Pictured</t>
+  </si>
+  <si>
+    <t>Downcomer Bottom</t>
+  </si>
+  <si>
+    <t>Versus Derived</t>
+  </si>
+  <si>
+    <t>Relative</t>
+  </si>
+  <si>
+    <t>Absolute</t>
+  </si>
+  <si>
+    <t>Consistency Checks (Pictured vs. Derived)</t>
+  </si>
+  <si>
+    <t>Cap Radii</t>
+  </si>
+  <si>
+    <t>Heater Box Bottom</t>
+  </si>
+  <si>
+    <t>Lower Plenum Bottom</t>
+  </si>
+  <si>
+    <t>Tee-Branch Top</t>
+  </si>
+  <si>
+    <t>Tee-Branch Bottom</t>
+  </si>
+  <si>
+    <t>Lower Plenum Top</t>
+  </si>
+  <si>
+    <t>Upper Plenum Bottom</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000000E+00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,12 +257,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,7 +287,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -186,7 +332,43 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thick">
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -195,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -203,25 +385,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -524,273 +745,581 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="7" max="8" width="7.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="2" style="1" customWidth="1"/>
+    <col min="2" max="3" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="3" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+    <row r="1" spans="2:12" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="G3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="K3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="8"/>
+    </row>
+    <row r="4" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="8"/>
+      <c r="K4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2">
+        <v>6.75</v>
+      </c>
+      <c r="E5" s="17">
+        <f>CONVERT(D5,"in","m")</f>
+        <v>0.17144999999999999</v>
+      </c>
+      <c r="G5" s="16"/>
+      <c r="H5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="4">
+        <v>2</v>
+      </c>
+      <c r="L5" s="4">
+        <f>CONVERT(K5,"in","m")</f>
+        <v>5.0799999999999998E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2">
+        <v>66.268000000000001</v>
+      </c>
+      <c r="E6" s="17">
+        <f>CONVERT(D6,"in","m")</f>
+        <v>1.6832072</v>
+      </c>
+      <c r="G6" s="2">
+        <v>60</v>
+      </c>
+      <c r="H6" s="2">
+        <f>38+D5</f>
+        <v>44.75</v>
+      </c>
+      <c r="I6" s="2">
+        <f>CONVERT(H6,"in","m")</f>
+        <v>1.1366499999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2">
+        <v>5.375</v>
+      </c>
+      <c r="E7" s="17">
+        <f>CONVERT(D7,"in","m")</f>
+        <v>0.13652500000000001</v>
+      </c>
+      <c r="G7" s="2">
+        <v>70</v>
+      </c>
+      <c r="H7" s="2">
+        <f>45.2+D5</f>
+        <v>51.95</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" ref="I7:I8" si="0">CONVERT(H7,"in","m")</f>
+        <v>1.3195300000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1">
+        <v>6.8209999999999997</v>
+      </c>
+      <c r="E8" s="17">
+        <f>CONVERT(D8,"in","m")</f>
+        <v>0.1732534</v>
+      </c>
+      <c r="G8" s="4">
+        <v>80</v>
+      </c>
+      <c r="H8" s="4">
+        <f>52.5+D5</f>
+        <v>59.25</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" si="0"/>
+        <v>1.50495</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="8"/>
+    </row>
+    <row r="9" spans="2:12" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="1">
+        <v>201.52699999999999</v>
+      </c>
+      <c r="E9" s="17">
+        <f>CONVERT(D9,"in","m")</f>
+        <v>5.1187858000000004</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="1">
+        <v>8.8049999999999997</v>
+      </c>
+      <c r="E10" s="17">
+        <f>CONVERT(D10,"in","m")</f>
+        <v>0.22364700000000001</v>
+      </c>
+      <c r="K10" s="4">
+        <v>158</v>
+      </c>
+      <c r="L10" s="4">
+        <f>CONVERT(CONVERT(CONVERT(K10,"in","m"),"in","m"),"in","m")</f>
+        <v>2.5891561120000004E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="2">
+        <f>10.236+2.687</f>
+        <v>12.923</v>
+      </c>
+      <c r="E11" s="17">
+        <f>CONVERT(D11,"in","m")</f>
+        <v>0.32824419999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="2">
+        <f>2.687</f>
+        <v>2.6869999999999998</v>
+      </c>
+      <c r="E12" s="17">
+        <f>CONVERT(D12,"in","m")</f>
+        <v>6.8249799999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="1">
+        <f>D12</f>
+        <v>2.6869999999999998</v>
+      </c>
+      <c r="E13" s="17">
+        <f>CONVERT(D13,"in","m")</f>
+        <v>6.8249799999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="2">
+        <v>6</v>
+      </c>
+      <c r="E14" s="17">
+        <f>CONVERT(D14,"in","m")</f>
+        <v>0.15240000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="4">
+        <v>22.727</v>
+      </c>
+      <c r="E15" s="18">
+        <f>CONVERT(D15,"in","m")</f>
+        <v>0.57726580000000005</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+    </row>
+    <row r="16" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="G18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18" s="1">
+        <f>195.117+5.69</f>
+        <v>200.80699999999999</v>
+      </c>
+      <c r="J18" s="1">
+        <f>CONVERT(I18,"in","m")</f>
+        <v>5.1004978000000003</v>
+      </c>
+      <c r="K18" s="14">
+        <f>ABS(I18-D26)</f>
+        <v>0.3200000000000216</v>
+      </c>
+      <c r="L18" s="14">
+        <f>K18/I18</f>
+        <v>1.5935699452709398E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C19" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D19" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="G3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7" t="s">
+      <c r="E19" s="8"/>
+      <c r="G19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="4">
+        <v>32.753</v>
+      </c>
+      <c r="J19" s="4">
+        <f>CONVERT(I19,"in","m")</f>
+        <v>0.83192619999999995</v>
+      </c>
+      <c r="K19" s="15">
+        <f>ABS(I19-D27)</f>
+        <v>1.4210854715202004E-14</v>
+      </c>
+      <c r="L19" s="15">
+        <f>K19/I19</f>
+        <v>4.338794832596099E-16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E20" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
+    </row>
+    <row r="21" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="19">
+        <f>4.026/2 + D8-2.687</f>
+        <v>6.1470000000000002</v>
+      </c>
+      <c r="E21" s="22">
+        <f>CONVERT(D21,"in","m")</f>
+        <v>0.15613379999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="20">
+        <f>SUM(D8:D10)</f>
+        <v>217.15299999999999</v>
+      </c>
+      <c r="E22" s="21">
+        <f>CONVERT(D22,"in","m")</f>
+        <v>5.5156862000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="2">
+        <f>D22+D15</f>
+        <v>239.88</v>
+      </c>
+      <c r="E23" s="17">
+        <f>CONVERT(D23,"in","m")</f>
+        <v>6.0929520000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D24" s="2">
+        <f>D23 - I19</f>
+        <v>207.12700000000001</v>
+      </c>
+      <c r="E24" s="17">
+        <f>CONVERT(D24,"in","m")</f>
+        <v>5.2610257999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="2">
+        <f>SUM(D12,D13,D9)</f>
+        <v>206.90099999999998</v>
+      </c>
+      <c r="E25" s="17">
+        <f>CONVERT(D25,"in","m")</f>
+        <v>5.2552853999999991</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="2">
+        <f>D24-D14</f>
+        <v>201.12700000000001</v>
+      </c>
+      <c r="E26" s="17">
+        <f>CONVERT(D26,"in","m")</f>
+        <v>5.1086258000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="2">
+        <f>D23-D24</f>
+        <v>32.752999999999986</v>
+      </c>
+      <c r="E27" s="17">
+        <f t="shared" ref="E27" si="1">CONVERT(D27,"in","m")</f>
+        <v>0.83192619999999962</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D28" s="4">
+        <f>SUM(D5:D7)</f>
         <v>78.393000000000001</v>
       </c>
-      <c r="E5" s="1">
-        <f>CONVERT(D5,"in","m")</f>
+      <c r="E28" s="18">
+        <f>CONVERT(D28,"in","m")</f>
         <v>1.9911821999999999</v>
       </c>
-      <c r="G5" s="9">
-        <v>2</v>
-      </c>
-      <c r="H5" s="9">
-        <f>CONVERT(G5,"in","m")</f>
-        <v>5.0799999999999998E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" ht="21.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="1">
-        <v>32.753</v>
-      </c>
-      <c r="E6" s="1">
-        <f>CONVERT(D6,"in","m")</f>
-        <v>0.83192619999999995</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="1">
-        <v>6.8209999999999997</v>
-      </c>
-      <c r="E7" s="1">
-        <f>CONVERT(D7,"in","m")</f>
-        <v>0.1732534</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="1">
-        <v>201.52699999999999</v>
-      </c>
-      <c r="E8" s="1">
-        <f>CONVERT(D8,"in","m")</f>
-        <v>5.1187858000000004</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="1">
-        <v>8.8049999999999997</v>
-      </c>
-      <c r="E9" s="1">
-        <f>CONVERT(D9,"in","m")</f>
-        <v>0.22364700000000001</v>
-      </c>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="2:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="8">
-        <v>22.727</v>
-      </c>
-      <c r="E10" s="8">
-        <f>CONVERT(D10,"in","m")</f>
-        <v>0.57726580000000005</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="1">
-        <f>SUM(D7:D10)</f>
-        <v>239.88</v>
-      </c>
-      <c r="E16" s="1">
-        <f>CONVERT(D16,"in","m")</f>
-        <v>6.0929520000000004</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="1">
-        <f>D16 - D6</f>
-        <v>207.12700000000001</v>
-      </c>
-      <c r="E17" s="1">
-        <f>CONVERT(D17,"in","m")</f>
-        <v>5.2610257999999996</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="8">
-        <f>SUM(D7:D9)</f>
-        <v>217.15299999999999</v>
-      </c>
-      <c r="E18" s="8">
-        <f>CONVERT(D18,"in","m")</f>
-        <v>5.5156862000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="29" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G7:H7"/>
+  <mergeCells count="18">
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="G15:L15"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K8:L8"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="G3:I3"/>
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="D16 D18" formulaRange="1"/>
+    <ignoredError sqref="D22 D28" formulaRange="1"/>
   </ignoredErrors>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Change: Adjusted Excel values for dimensioning
</commit_message>
<xml_diff>
--- a/Dimensions/Dimensions.xlsx
+++ b/Dimensions/Dimensions.xlsx
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="37">
   <si>
     <t>From</t>
   </si>
@@ -221,16 +221,22 @@
     <t>Lower Plenum Bottom</t>
   </si>
   <si>
-    <t>Tee-Branch Top</t>
-  </si>
-  <si>
-    <t>Tee-Branch Bottom</t>
-  </si>
-  <si>
     <t>Lower Plenum Top</t>
   </si>
   <si>
     <t>Upper Plenum Bottom</t>
+  </si>
+  <si>
+    <t>Upper Plenum  Bottom</t>
+  </si>
+  <si>
+    <t>Upper Plenum Top</t>
+  </si>
+  <si>
+    <t>Chimney Bottom</t>
+  </si>
+  <si>
+    <t>Chimney Top</t>
   </si>
 </sst>
 </file>
@@ -746,16 +752,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L29"/>
+  <dimension ref="B1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" style="1" customWidth="1"/>
-    <col min="2" max="3" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="3" style="1" customWidth="1"/>
@@ -1006,50 +1013,36 @@
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="1">
-        <f>D12</f>
-        <v>2.6869999999999998</v>
+      <c r="B13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="2">
+        <v>6</v>
       </c>
       <c r="E13" s="17">
         <f>CONVERT(D13,"in","m")</f>
-        <v>6.8249799999999999E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="2">
-        <v>6</v>
-      </c>
-      <c r="E14" s="17">
+        <v>0.15240000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="4">
+        <v>22.727</v>
+      </c>
+      <c r="E14" s="18">
         <f>CONVERT(D14,"in","m")</f>
-        <v>0.15240000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="4">
-        <v>22.727</v>
-      </c>
-      <c r="E15" s="18">
-        <f>CONVERT(D15,"in","m")</f>
         <v>0.57726580000000005</v>
       </c>
+    </row>
+    <row r="15" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G15" s="11" t="s">
         <v>27</v>
       </c>
@@ -1075,7 +1068,13 @@
       </c>
       <c r="L16" s="8"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="5" t="s">
@@ -1091,13 +1090,17 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
+    <row r="18" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="8"/>
       <c r="G18" s="1" t="s">
         <v>23</v>
       </c>
@@ -1113,7 +1116,7 @@
         <v>5.1004978000000003</v>
       </c>
       <c r="K18" s="14">
-        <f>ABS(I18-D26)</f>
+        <f>ABS(I18-D29)</f>
         <v>0.3200000000000216</v>
       </c>
       <c r="L18" s="14">
@@ -1121,17 +1124,15 @@
         <v>1.5935699452709398E-3</v>
       </c>
     </row>
-    <row r="19" spans="2:12" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="8"/>
+    <row r="19" spans="2:12" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="G19" s="4" t="s">
         <v>4</v>
       </c>
@@ -1146,7 +1147,7 @@
         <v>0.83192619999999995</v>
       </c>
       <c r="K19" s="15">
-        <f>ABS(I19-D27)</f>
+        <f>ABS(I19-D30)</f>
         <v>1.4210854715202004E-14</v>
       </c>
       <c r="L19" s="15">
@@ -1155,45 +1156,51 @@
       </c>
     </row>
     <row r="20" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>2</v>
+      <c r="B20" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="19">
+        <f>4.026/2 + D8-D12</f>
+        <v>6.1470000000000002</v>
+      </c>
+      <c r="E20" s="22">
+        <f>CONVERT(D20,"in","m")</f>
+        <v>0.15613379999999999</v>
       </c>
     </row>
     <row r="21" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="19">
-        <f>4.026/2 + D8-2.687</f>
-        <v>6.1470000000000002</v>
-      </c>
-      <c r="E21" s="22">
+      <c r="B21" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="20">
+        <f>SUM(D8:D10)</f>
+        <v>217.15299999999999</v>
+      </c>
+      <c r="E21" s="21">
         <f>CONVERT(D21,"in","m")</f>
-        <v>0.15613379999999999</v>
+        <v>5.5156862000000002</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="20" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="D22" s="20">
-        <f>SUM(D8:D10)</f>
-        <v>217.15299999999999</v>
+        <f>D21+4.026</f>
+        <v>221.179</v>
       </c>
       <c r="E22" s="21">
         <f>CONVERT(D22,"in","m")</f>
-        <v>5.5156862000000002</v>
+        <v>5.6179465999999998</v>
       </c>
     </row>
     <row r="23" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1204,7 +1211,7 @@
         <v>12</v>
       </c>
       <c r="D23" s="2">
-        <f>D22+D15</f>
+        <f>D21+D14</f>
         <v>239.88</v>
       </c>
       <c r="E23" s="17">
@@ -1227,72 +1234,132 @@
         <f>CONVERT(D24,"in","m")</f>
         <v>5.2610257999999996</v>
       </c>
+      <c r="G24" s="17">
+        <f>E28/10</f>
+        <v>2.7246579999999999E-2</v>
+      </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D25" s="2">
-        <f>SUM(D12,D13,D9)</f>
-        <v>206.90099999999998</v>
+        <f>D11 + D12</f>
+        <v>15.61</v>
       </c>
       <c r="E25" s="17">
         <f>CONVERT(D25,"in","m")</f>
-        <v>5.2552853999999991</v>
+        <v>0.39649400000000001</v>
+      </c>
+      <c r="G25" s="17">
+        <f>G24*0.008213057</f>
+        <v>2.2377771459505997E-4</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="2">
-        <f>D24-D14</f>
-        <v>201.12700000000001</v>
+      <c r="B26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="1">
+        <f>D12+2.125</f>
+        <v>4.8119999999999994</v>
       </c>
       <c r="E26" s="17">
         <f>CONVERT(D26,"in","m")</f>
-        <v>5.1086258000000004</v>
+        <v>0.12222479999999998</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="2">
+        <f>SUM(D12,D26,D9)</f>
+        <v>209.02599999999998</v>
+      </c>
+      <c r="E27" s="17">
+        <f>CONVERT(D27,"in","m")</f>
+        <v>5.3092603999999994</v>
+      </c>
+      <c r="G27" s="17">
+        <f>0.4070604+G24</f>
+        <v>0.43430698000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="2">
+        <f>D14-12</f>
+        <v>10.727</v>
+      </c>
+      <c r="E28" s="17">
+        <f>CONVERT(D28,"in","m")</f>
+        <v>0.27246579999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D29" s="2">
+        <f>D24-D13</f>
+        <v>201.12700000000001</v>
+      </c>
+      <c r="E29" s="17">
+        <f>CONVERT(D29,"in","m")</f>
+        <v>5.1086258000000004</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D30" s="2">
         <f>D23-D24</f>
         <v>32.752999999999986</v>
       </c>
-      <c r="E27" s="17">
-        <f t="shared" ref="E27" si="1">CONVERT(D27,"in","m")</f>
+      <c r="E30" s="17">
+        <f t="shared" ref="E30" si="1">CONVERT(D30,"in","m")</f>
         <v>0.83192619999999962</v>
       </c>
     </row>
-    <row r="28" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="4" t="s">
+    <row r="31" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D31" s="4">
         <f>SUM(D5:D7)</f>
         <v>78.393000000000001</v>
       </c>
-      <c r="E28" s="18">
-        <f>CONVERT(D28,"in","m")</f>
+      <c r="E31" s="18">
+        <f>CONVERT(D31,"in","m")</f>
         <v>1.9911821999999999</v>
       </c>
     </row>
-    <row r="29" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="18">
     <mergeCell ref="G16:G17"/>
@@ -1305,10 +1372,10 @@
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="D18:E18"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="G3:I3"/>
     <mergeCell ref="B2:E2"/>
@@ -1317,7 +1384,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="D22 D28" formulaRange="1"/>
+    <ignoredError sqref="D21 D31" formulaRange="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>

</xml_diff>